<commit_message>
one more ordering fix
</commit_message>
<xml_diff>
--- a/rapid/rapid_spending.xlsx
+++ b/rapid/rapid_spending.xlsx
@@ -527,13 +527,13 @@
     <t xml:space="preserve">Provision of insecticide nets</t>
   </si>
   <si>
+    <t xml:space="preserve">Psychological and antidepressant therapy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Psychological treatment</t>
   </si>
   <si>
     <t xml:space="preserve">Psychosocial support and counseling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psychological and antidepressant therapy</t>
   </si>
   <si>
     <t xml:space="preserve">Referral for DST and MDR-TB treatment</t>
@@ -834,13 +834,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -851,6 +844,13 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -919,7 +919,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -929,19 +929,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -949,19 +949,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -981,7 +981,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -993,7 +993,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1095,13 +1095,13 @@
   <dimension ref="A1:AN194"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>